<commit_message>
feature: download all pregame reports for tstate
</commit_message>
<xml_diff>
--- a/core/report/game_report_template.xlsx
+++ b/core/report/game_report_template.xlsx
@@ -15,7 +15,7 @@
     <sheet name="DBT" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">DBT!$A$1:$V$58</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">DBT!$A$1:$V$57</definedName>
   </definedNames>
   <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
@@ -1113,6 +1113,72 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="50" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1122,9 +1188,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="47" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -1142,69 +1205,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1564,8 +1564,8 @@
   </sheetPr>
   <dimension ref="A1:V57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A36" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
-      <selection activeCell="J33" sqref="J33"/>
+    <sheetView tabSelected="1" zoomScale="88" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
+      <selection activeCell="X44" sqref="X44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1610,12 +1610,12 @@
       <c r="V2" s="3"/>
     </row>
     <row r="3" spans="1:22" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B3" s="94" t="s">
+      <c r="B3" s="115" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="95"/>
-      <c r="D3" s="95"/>
-      <c r="E3" s="96"/>
+      <c r="C3" s="116"/>
+      <c r="D3" s="116"/>
+      <c r="E3" s="117"/>
       <c r="F3" s="4"/>
       <c r="G3" s="5" t="s">
         <v>2</v>
@@ -1645,10 +1645,10 @@
       <c r="V3" s="5"/>
     </row>
     <row r="4" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="B4" s="95"/>
-      <c r="C4" s="95"/>
-      <c r="D4" s="95"/>
-      <c r="E4" s="96"/>
+      <c r="B4" s="116"/>
+      <c r="C4" s="116"/>
+      <c r="D4" s="116"/>
+      <c r="E4" s="117"/>
       <c r="F4" s="4"/>
       <c r="G4" s="5" t="s">
         <v>7</v>
@@ -1676,10 +1676,10 @@
       <c r="V4" s="12"/>
     </row>
     <row r="5" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="B5" s="95"/>
-      <c r="C5" s="95"/>
-      <c r="D5" s="95"/>
-      <c r="E5" s="96"/>
+      <c r="B5" s="116"/>
+      <c r="C5" s="116"/>
+      <c r="D5" s="116"/>
+      <c r="E5" s="117"/>
       <c r="F5" s="4"/>
       <c r="G5" s="5" t="s">
         <v>11</v>
@@ -1761,21 +1761,21 @@
       <c r="V7" s="8"/>
     </row>
     <row r="8" spans="1:22" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B8" s="97"/>
-      <c r="C8" s="98"/>
-      <c r="D8" s="98"/>
-      <c r="E8" s="98"/>
-      <c r="F8" s="99"/>
-      <c r="G8" s="97"/>
-      <c r="H8" s="98"/>
-      <c r="I8" s="98"/>
-      <c r="J8" s="98"/>
-      <c r="K8" s="98"/>
-      <c r="L8" s="98"/>
-      <c r="M8" s="98"/>
-      <c r="N8" s="98"/>
-      <c r="O8" s="98"/>
-      <c r="P8" s="99"/>
+      <c r="B8" s="118"/>
+      <c r="C8" s="119"/>
+      <c r="D8" s="119"/>
+      <c r="E8" s="119"/>
+      <c r="F8" s="120"/>
+      <c r="G8" s="118"/>
+      <c r="H8" s="119"/>
+      <c r="I8" s="119"/>
+      <c r="J8" s="119"/>
+      <c r="K8" s="119"/>
+      <c r="L8" s="119"/>
+      <c r="M8" s="119"/>
+      <c r="N8" s="119"/>
+      <c r="O8" s="119"/>
+      <c r="P8" s="120"/>
       <c r="Q8" s="9">
         <v>1</v>
       </c>
@@ -1789,25 +1789,25 @@
       <c r="B9" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="C9" s="93" t="s">
+      <c r="C9" s="99" t="s">
         <v>19</v>
       </c>
-      <c r="D9" s="93"/>
-      <c r="E9" s="93"/>
-      <c r="F9" s="93" t="s">
+      <c r="D9" s="99"/>
+      <c r="E9" s="99"/>
+      <c r="F9" s="99" t="s">
         <v>20</v>
       </c>
-      <c r="G9" s="93"/>
-      <c r="H9" s="93"/>
-      <c r="I9" s="93" t="s">
+      <c r="G9" s="99"/>
+      <c r="H9" s="99"/>
+      <c r="I9" s="99" t="s">
         <v>21</v>
       </c>
-      <c r="J9" s="93"/>
-      <c r="K9" s="93"/>
-      <c r="L9" s="93" t="s">
+      <c r="J9" s="99"/>
+      <c r="K9" s="99"/>
+      <c r="L9" s="99" t="s">
         <v>22</v>
       </c>
-      <c r="M9" s="93"/>
+      <c r="M9" s="99"/>
       <c r="N9" s="17" t="s">
         <v>23</v>
       </c>
@@ -1824,12 +1824,12 @@
     </row>
     <row r="10" spans="1:22" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B10" s="4"/>
-      <c r="C10" s="97"/>
-      <c r="D10" s="98"/>
-      <c r="E10" s="99"/>
-      <c r="F10" s="97"/>
-      <c r="G10" s="98"/>
-      <c r="H10" s="99"/>
+      <c r="C10" s="118"/>
+      <c r="D10" s="119"/>
+      <c r="E10" s="120"/>
+      <c r="F10" s="118"/>
+      <c r="G10" s="119"/>
+      <c r="H10" s="120"/>
       <c r="I10" s="23"/>
       <c r="J10" s="24"/>
       <c r="K10" s="25"/>
@@ -1871,22 +1871,22 @@
       <c r="H12" s="28" t="s">
         <v>29</v>
       </c>
-      <c r="J12" s="90" t="s">
+      <c r="J12" s="112" t="s">
         <v>36</v>
       </c>
-      <c r="K12" s="91"/>
-      <c r="L12" s="91"/>
-      <c r="M12" s="91"/>
-      <c r="N12" s="91"/>
-      <c r="O12" s="92"/>
-      <c r="Q12" s="90" t="s">
+      <c r="K12" s="113"/>
+      <c r="L12" s="113"/>
+      <c r="M12" s="113"/>
+      <c r="N12" s="113"/>
+      <c r="O12" s="114"/>
+      <c r="Q12" s="112" t="s">
         <v>38</v>
       </c>
-      <c r="R12" s="91"/>
-      <c r="S12" s="91"/>
-      <c r="T12" s="91"/>
-      <c r="U12" s="91"/>
-      <c r="V12" s="92"/>
+      <c r="R12" s="113"/>
+      <c r="S12" s="113"/>
+      <c r="T12" s="113"/>
+      <c r="U12" s="113"/>
+      <c r="V12" s="114"/>
     </row>
     <row r="13" spans="1:22" ht="14.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A13" s="28"/>
@@ -2347,11 +2347,11 @@
       <c r="V26" s="70"/>
     </row>
     <row r="27" spans="1:22" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="100" t="s">
+      <c r="A27" s="103" t="s">
         <v>33</v>
       </c>
-      <c r="B27" s="101"/>
-      <c r="C27" s="102"/>
+      <c r="B27" s="104"/>
+      <c r="C27" s="105"/>
       <c r="D27" s="30" t="s">
         <v>34</v>
       </c>
@@ -2722,24 +2722,24 @@
       <c r="F40" s="36"/>
       <c r="G40" s="36"/>
       <c r="H40" s="36"/>
-      <c r="J40" s="103" t="s">
+      <c r="J40" s="111" t="s">
         <v>36</v>
       </c>
-      <c r="K40" s="104"/>
-      <c r="L40" s="105"/>
+      <c r="K40" s="107"/>
+      <c r="L40" s="108"/>
       <c r="M40" s="42"/>
-      <c r="N40" s="104" t="s">
+      <c r="N40" s="107" t="s">
         <v>37</v>
       </c>
       <c r="O40" s="43"/>
       <c r="P40" s="44"/>
-      <c r="Q40" s="109" t="s">
+      <c r="Q40" s="110" t="s">
         <v>38</v>
       </c>
-      <c r="R40" s="104"/>
-      <c r="S40" s="105"/>
+      <c r="R40" s="107"/>
+      <c r="S40" s="108"/>
       <c r="T40" s="42"/>
-      <c r="U40" s="104" t="s">
+      <c r="U40" s="107" t="s">
         <v>37</v>
       </c>
       <c r="V40" s="45"/>
@@ -2755,18 +2755,18 @@
       <c r="F41" s="28"/>
       <c r="G41" s="28"/>
       <c r="H41" s="28"/>
-      <c r="J41" s="106"/>
-      <c r="K41" s="107"/>
-      <c r="L41" s="108"/>
+      <c r="J41" s="109"/>
+      <c r="K41" s="94"/>
+      <c r="L41" s="95"/>
       <c r="M41" s="21"/>
-      <c r="N41" s="107"/>
+      <c r="N41" s="94"/>
       <c r="O41" s="22"/>
       <c r="P41" s="9"/>
-      <c r="Q41" s="110"/>
-      <c r="R41" s="107"/>
-      <c r="S41" s="108"/>
+      <c r="Q41" s="93"/>
+      <c r="R41" s="94"/>
+      <c r="S41" s="95"/>
       <c r="T41" s="21"/>
-      <c r="U41" s="107"/>
+      <c r="U41" s="94"/>
       <c r="V41" s="46"/>
     </row>
     <row r="42" spans="1:22" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
@@ -2780,24 +2780,24 @@
       <c r="F42" s="28"/>
       <c r="G42" s="28"/>
       <c r="H42" s="28"/>
-      <c r="J42" s="115" t="s">
+      <c r="J42" s="97" t="s">
         <v>39</v>
       </c>
-      <c r="K42" s="112"/>
-      <c r="L42" s="113"/>
+      <c r="K42" s="91"/>
+      <c r="L42" s="92"/>
       <c r="M42" s="10"/>
-      <c r="N42" s="112" t="s">
+      <c r="N42" s="91" t="s">
         <v>37</v>
       </c>
       <c r="O42" s="20"/>
       <c r="P42" s="9"/>
-      <c r="Q42" s="111" t="s">
+      <c r="Q42" s="90" t="s">
         <v>39</v>
       </c>
-      <c r="R42" s="112"/>
-      <c r="S42" s="113"/>
+      <c r="R42" s="91"/>
+      <c r="S42" s="92"/>
       <c r="T42" s="10"/>
-      <c r="U42" s="112" t="s">
+      <c r="U42" s="91" t="s">
         <v>37</v>
       </c>
       <c r="V42" s="47"/>
@@ -2813,26 +2813,26 @@
       <c r="F43" s="28"/>
       <c r="G43" s="28"/>
       <c r="H43" s="28"/>
-      <c r="J43" s="116"/>
-      <c r="K43" s="93"/>
-      <c r="L43" s="117"/>
+      <c r="J43" s="98"/>
+      <c r="K43" s="99"/>
+      <c r="L43" s="100"/>
       <c r="M43" s="21"/>
-      <c r="N43" s="118"/>
+      <c r="N43" s="101"/>
       <c r="O43" s="22"/>
       <c r="P43" s="9"/>
-      <c r="Q43" s="119"/>
-      <c r="R43" s="93"/>
-      <c r="S43" s="117"/>
+      <c r="Q43" s="102"/>
+      <c r="R43" s="99"/>
+      <c r="S43" s="100"/>
       <c r="T43" s="21"/>
-      <c r="U43" s="118"/>
+      <c r="U43" s="101"/>
       <c r="V43" s="46"/>
     </row>
     <row r="44" spans="1:22" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A44" s="100" t="s">
+      <c r="A44" s="103" t="s">
         <v>33</v>
       </c>
-      <c r="B44" s="101"/>
-      <c r="C44" s="102"/>
+      <c r="B44" s="104"/>
+      <c r="C44" s="105"/>
       <c r="D44" s="30" t="s">
         <v>34</v>
       </c>
@@ -2840,22 +2840,22 @@
       <c r="F44" s="30"/>
       <c r="G44" s="29"/>
       <c r="H44" s="30"/>
-      <c r="J44" s="120" t="s">
+      <c r="J44" s="106" t="s">
         <v>40</v>
       </c>
-      <c r="K44" s="104"/>
-      <c r="L44" s="104"/>
-      <c r="M44" s="104"/>
-      <c r="N44" s="104"/>
-      <c r="O44" s="105"/>
+      <c r="K44" s="107"/>
+      <c r="L44" s="107"/>
+      <c r="M44" s="107"/>
+      <c r="N44" s="107"/>
+      <c r="O44" s="108"/>
       <c r="P44" s="44"/>
-      <c r="Q44" s="109" t="s">
+      <c r="Q44" s="110" t="s">
         <v>41</v>
       </c>
-      <c r="R44" s="104"/>
-      <c r="S44" s="105"/>
+      <c r="R44" s="107"/>
+      <c r="S44" s="108"/>
       <c r="T44" s="42"/>
-      <c r="U44" s="104" t="s">
+      <c r="U44" s="107" t="s">
         <v>37</v>
       </c>
       <c r="V44" s="45"/>
@@ -2869,18 +2869,18 @@
       <c r="F45" s="31"/>
       <c r="G45" s="31"/>
       <c r="H45" s="31"/>
-      <c r="J45" s="106"/>
-      <c r="K45" s="107"/>
-      <c r="L45" s="107"/>
-      <c r="M45" s="107"/>
-      <c r="N45" s="107"/>
-      <c r="O45" s="108"/>
+      <c r="J45" s="109"/>
+      <c r="K45" s="94"/>
+      <c r="L45" s="94"/>
+      <c r="M45" s="94"/>
+      <c r="N45" s="94"/>
+      <c r="O45" s="95"/>
       <c r="P45" s="9"/>
-      <c r="Q45" s="110"/>
-      <c r="R45" s="107"/>
-      <c r="S45" s="108"/>
+      <c r="Q45" s="93"/>
+      <c r="R45" s="94"/>
+      <c r="S45" s="95"/>
       <c r="T45" s="21"/>
-      <c r="U45" s="107"/>
+      <c r="U45" s="94"/>
       <c r="V45" s="46"/>
     </row>
     <row r="46" spans="1:22" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
@@ -2891,13 +2891,13 @@
       <c r="N46" s="19"/>
       <c r="O46" s="19"/>
       <c r="P46" s="20"/>
-      <c r="Q46" s="111" t="s">
+      <c r="Q46" s="90" t="s">
         <v>39</v>
       </c>
-      <c r="R46" s="112"/>
-      <c r="S46" s="113"/>
+      <c r="R46" s="91"/>
+      <c r="S46" s="92"/>
       <c r="T46" s="19"/>
-      <c r="U46" s="112" t="s">
+      <c r="U46" s="91" t="s">
         <v>37</v>
       </c>
       <c r="V46" s="47"/>
@@ -2906,16 +2906,16 @@
       <c r="B47" t="s">
         <v>42</v>
       </c>
-      <c r="C47" s="114" t="s">
+      <c r="C47" s="96" t="s">
         <v>43</v>
       </c>
-      <c r="D47" s="114"/>
-      <c r="E47" s="114" t="s">
+      <c r="D47" s="96"/>
+      <c r="E47" s="96" t="s">
         <v>44</v>
       </c>
-      <c r="F47" s="114"/>
-      <c r="G47" s="114"/>
-      <c r="H47" s="114"/>
+      <c r="F47" s="96"/>
+      <c r="G47" s="96"/>
+      <c r="H47" s="96"/>
       <c r="J47" s="51" t="s">
         <v>45</v>
       </c>
@@ -2925,11 +2925,11 @@
       <c r="N47" s="26"/>
       <c r="O47" s="26"/>
       <c r="P47" s="27"/>
-      <c r="Q47" s="110"/>
-      <c r="R47" s="107"/>
-      <c r="S47" s="108"/>
+      <c r="Q47" s="93"/>
+      <c r="R47" s="94"/>
+      <c r="S47" s="95"/>
       <c r="T47" s="26"/>
-      <c r="U47" s="107"/>
+      <c r="U47" s="94"/>
       <c r="V47" s="52"/>
     </row>
     <row r="48" spans="1:22" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
@@ -3179,6 +3179,22 @@
     </row>
   </sheetData>
   <mergeCells count="28">
+    <mergeCell ref="J12:O12"/>
+    <mergeCell ref="Q12:V12"/>
+    <mergeCell ref="L9:M9"/>
+    <mergeCell ref="B3:E5"/>
+    <mergeCell ref="B8:F8"/>
+    <mergeCell ref="C9:E9"/>
+    <mergeCell ref="F9:H9"/>
+    <mergeCell ref="I9:K9"/>
+    <mergeCell ref="G8:P8"/>
+    <mergeCell ref="C10:E10"/>
+    <mergeCell ref="F10:H10"/>
+    <mergeCell ref="A27:C27"/>
+    <mergeCell ref="J40:L41"/>
+    <mergeCell ref="N40:N41"/>
+    <mergeCell ref="Q40:S41"/>
+    <mergeCell ref="U40:U41"/>
     <mergeCell ref="Q46:S47"/>
     <mergeCell ref="U46:U47"/>
     <mergeCell ref="C47:D47"/>
@@ -3191,25 +3207,9 @@
     <mergeCell ref="J44:O45"/>
     <mergeCell ref="Q44:S45"/>
     <mergeCell ref="U44:U45"/>
-    <mergeCell ref="A27:C27"/>
-    <mergeCell ref="J40:L41"/>
-    <mergeCell ref="N40:N41"/>
-    <mergeCell ref="Q40:S41"/>
-    <mergeCell ref="U40:U41"/>
-    <mergeCell ref="J12:O12"/>
-    <mergeCell ref="Q12:V12"/>
-    <mergeCell ref="L9:M9"/>
-    <mergeCell ref="B3:E5"/>
-    <mergeCell ref="B8:F8"/>
-    <mergeCell ref="C9:E9"/>
-    <mergeCell ref="F9:H9"/>
-    <mergeCell ref="I9:K9"/>
-    <mergeCell ref="G8:P8"/>
-    <mergeCell ref="C10:E10"/>
-    <mergeCell ref="F10:H10"/>
   </mergeCells>
   <pageMargins left="0" right="0" top="0.39370078740157483" bottom="0.39370078740157483" header="0.51181102362204722" footer="0.51181102362204722"/>
-  <pageSetup paperSize="9" scale="94" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
game_report adapted player list
</commit_message>
<xml_diff>
--- a/core/report/game_report_template.xlsx
+++ b/core/report/game_report_template.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="59">
   <si>
     <r>
       <rPr>
@@ -135,9 +135,6 @@
     <t>B</t>
   </si>
   <si>
-    <t>C</t>
-  </si>
-  <si>
     <t>Unterschrift Off. A</t>
   </si>
   <si>
@@ -159,10 +156,6 @@
     <t>Satzpunkte</t>
   </si>
   <si>
-    <t>Einer gegen den Torwart
-''Shoot-out'</t>
-  </si>
-  <si>
     <t>3. Satz</t>
   </si>
   <si>
@@ -215,6 +208,13 @@
   </si>
   <si>
     <t>'Golden Goal'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Einer gegen den Torwart
+</t>
+  </si>
+  <si>
+    <t>'Shoot-out'</t>
   </si>
 </sst>
 </file>
@@ -431,49 +431,8 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thick">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right/>
-      <top style="thick">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
-      <top style="thick">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
       <top style="thick">
         <color auto="1"/>
       </top>
@@ -898,11 +857,50 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thick">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thick">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="121">
+  <cellXfs count="122">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -985,62 +983,67 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -1054,15 +1057,6 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="41" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="42" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="43" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1071,48 +1065,53 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="41" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="47" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="45" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="48" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="49" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="50" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="46" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="47" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="51" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="52" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="53" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="49" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="50" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1134,21 +1133,21 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1162,30 +1161,30 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="46" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="43" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="47" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1227,16 +1226,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>228600</xdr:colOff>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>63502</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>20</xdr:col>
-      <xdr:colOff>25400</xdr:colOff>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>189557</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>127000</xdr:rowOff>
+      <xdr:rowOff>132772</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1245,7 +1244,7 @@
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
-      <xdr:blipFill>
+      <xdr:blipFill rotWithShape="1">
         <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="hqprint">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
@@ -1253,15 +1252,13 @@
             </a:ext>
           </a:extLst>
         </a:blip>
-        <a:srcRect/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
+        <a:srcRect l="6493" t="5608" r="7771" b="8496"/>
+        <a:stretch/>
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="6451600" y="0"/>
-          <a:ext cx="635000" cy="647700"/>
+          <a:off x="6044047" y="0"/>
+          <a:ext cx="622510" cy="646545"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1562,10 +1559,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:V57"/>
+  <dimension ref="A1:X57"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="88" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
-      <selection activeCell="X44" sqref="X44"/>
+    <sheetView tabSelected="1" topLeftCell="L1" zoomScale="165" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
+      <selection activeCell="X3" sqref="X3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1610,12 +1607,12 @@
       <c r="V2" s="3"/>
     </row>
     <row r="3" spans="1:22" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B3" s="115" t="s">
+      <c r="B3" s="116" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="116"/>
-      <c r="D3" s="116"/>
-      <c r="E3" s="117"/>
+      <c r="C3" s="117"/>
+      <c r="D3" s="117"/>
+      <c r="E3" s="118"/>
       <c r="F3" s="4"/>
       <c r="G3" s="5" t="s">
         <v>2</v>
@@ -1645,10 +1642,10 @@
       <c r="V3" s="5"/>
     </row>
     <row r="4" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="B4" s="116"/>
-      <c r="C4" s="116"/>
-      <c r="D4" s="116"/>
-      <c r="E4" s="117"/>
+      <c r="B4" s="117"/>
+      <c r="C4" s="117"/>
+      <c r="D4" s="117"/>
+      <c r="E4" s="118"/>
       <c r="F4" s="4"/>
       <c r="G4" s="5" t="s">
         <v>7</v>
@@ -1676,10 +1673,10 @@
       <c r="V4" s="12"/>
     </row>
     <row r="5" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="B5" s="116"/>
-      <c r="C5" s="116"/>
-      <c r="D5" s="116"/>
-      <c r="E5" s="117"/>
+      <c r="B5" s="117"/>
+      <c r="C5" s="117"/>
+      <c r="D5" s="117"/>
+      <c r="E5" s="118"/>
       <c r="F5" s="4"/>
       <c r="G5" s="5" t="s">
         <v>11</v>
@@ -1761,21 +1758,21 @@
       <c r="V7" s="8"/>
     </row>
     <row r="8" spans="1:22" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B8" s="118"/>
-      <c r="C8" s="119"/>
-      <c r="D8" s="119"/>
-      <c r="E8" s="119"/>
-      <c r="F8" s="120"/>
-      <c r="G8" s="118"/>
-      <c r="H8" s="119"/>
-      <c r="I8" s="119"/>
-      <c r="J8" s="119"/>
-      <c r="K8" s="119"/>
-      <c r="L8" s="119"/>
-      <c r="M8" s="119"/>
-      <c r="N8" s="119"/>
-      <c r="O8" s="119"/>
-      <c r="P8" s="120"/>
+      <c r="B8" s="119"/>
+      <c r="C8" s="120"/>
+      <c r="D8" s="120"/>
+      <c r="E8" s="120"/>
+      <c r="F8" s="121"/>
+      <c r="G8" s="119"/>
+      <c r="H8" s="120"/>
+      <c r="I8" s="120"/>
+      <c r="J8" s="120"/>
+      <c r="K8" s="120"/>
+      <c r="L8" s="120"/>
+      <c r="M8" s="120"/>
+      <c r="N8" s="120"/>
+      <c r="O8" s="120"/>
+      <c r="P8" s="121"/>
       <c r="Q8" s="9">
         <v>1</v>
       </c>
@@ -1789,25 +1786,25 @@
       <c r="B9" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="C9" s="99" t="s">
+      <c r="C9" s="100" t="s">
         <v>19</v>
       </c>
-      <c r="D9" s="99"/>
-      <c r="E9" s="99"/>
-      <c r="F9" s="99" t="s">
+      <c r="D9" s="100"/>
+      <c r="E9" s="100"/>
+      <c r="F9" s="100" t="s">
         <v>20</v>
       </c>
-      <c r="G9" s="99"/>
-      <c r="H9" s="99"/>
-      <c r="I9" s="99" t="s">
+      <c r="G9" s="100"/>
+      <c r="H9" s="100"/>
+      <c r="I9" s="100" t="s">
         <v>21</v>
       </c>
-      <c r="J9" s="99"/>
-      <c r="K9" s="99"/>
-      <c r="L9" s="99" t="s">
+      <c r="J9" s="100"/>
+      <c r="K9" s="100"/>
+      <c r="L9" s="100" t="s">
         <v>22</v>
       </c>
-      <c r="M9" s="99"/>
+      <c r="M9" s="100"/>
       <c r="N9" s="17" t="s">
         <v>23</v>
       </c>
@@ -1824,12 +1821,12 @@
     </row>
     <row r="10" spans="1:22" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B10" s="4"/>
-      <c r="C10" s="118"/>
-      <c r="D10" s="119"/>
-      <c r="E10" s="120"/>
-      <c r="F10" s="118"/>
-      <c r="G10" s="119"/>
-      <c r="H10" s="120"/>
+      <c r="C10" s="119"/>
+      <c r="D10" s="120"/>
+      <c r="E10" s="121"/>
+      <c r="F10" s="119"/>
+      <c r="G10" s="120"/>
+      <c r="H10" s="121"/>
       <c r="I10" s="23"/>
       <c r="J10" s="24"/>
       <c r="K10" s="25"/>
@@ -1871,22 +1868,22 @@
       <c r="H12" s="28" t="s">
         <v>29</v>
       </c>
-      <c r="J12" s="112" t="s">
-        <v>36</v>
-      </c>
-      <c r="K12" s="113"/>
-      <c r="L12" s="113"/>
-      <c r="M12" s="113"/>
-      <c r="N12" s="113"/>
-      <c r="O12" s="114"/>
-      <c r="Q12" s="112" t="s">
-        <v>38</v>
-      </c>
-      <c r="R12" s="113"/>
-      <c r="S12" s="113"/>
-      <c r="T12" s="113"/>
-      <c r="U12" s="113"/>
-      <c r="V12" s="114"/>
+      <c r="J12" s="113" t="s">
+        <v>35</v>
+      </c>
+      <c r="K12" s="114"/>
+      <c r="L12" s="114"/>
+      <c r="M12" s="114"/>
+      <c r="N12" s="114"/>
+      <c r="O12" s="115"/>
+      <c r="Q12" s="113" t="s">
+        <v>37</v>
+      </c>
+      <c r="R12" s="114"/>
+      <c r="S12" s="114"/>
+      <c r="T12" s="114"/>
+      <c r="U12" s="114"/>
+      <c r="V12" s="115"/>
     </row>
     <row r="13" spans="1:22" ht="14.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A13" s="28"/>
@@ -1897,41 +1894,41 @@
       <c r="F13" s="28"/>
       <c r="G13" s="28"/>
       <c r="H13" s="28"/>
-      <c r="J13" s="72" t="s">
+      <c r="J13" s="68" t="s">
         <v>30</v>
       </c>
-      <c r="K13" s="73" t="s">
+      <c r="K13" s="69" t="s">
         <v>26</v>
       </c>
-      <c r="L13" s="74" t="s">
+      <c r="L13" s="70" t="s">
         <v>31</v>
       </c>
-      <c r="M13" s="82" t="s">
+      <c r="M13" s="78" t="s">
         <v>30</v>
       </c>
-      <c r="N13" s="75" t="s">
+      <c r="N13" s="71" t="s">
         <v>26</v>
       </c>
-      <c r="O13" s="76" t="s">
+      <c r="O13" s="72" t="s">
         <v>31</v>
       </c>
       <c r="P13" s="31"/>
-      <c r="Q13" s="72" t="s">
+      <c r="Q13" s="68" t="s">
         <v>30</v>
       </c>
-      <c r="R13" s="73" t="s">
+      <c r="R13" s="69" t="s">
         <v>26</v>
       </c>
-      <c r="S13" s="74" t="s">
+      <c r="S13" s="70" t="s">
         <v>31</v>
       </c>
-      <c r="T13" s="82" t="s">
+      <c r="T13" s="78" t="s">
         <v>30</v>
       </c>
-      <c r="U13" s="75" t="s">
+      <c r="U13" s="71" t="s">
         <v>26</v>
       </c>
-      <c r="V13" s="76" t="s">
+      <c r="V13" s="72" t="s">
         <v>31</v>
       </c>
     </row>
@@ -1944,27 +1941,27 @@
       <c r="F14" s="28"/>
       <c r="G14" s="28"/>
       <c r="H14" s="28"/>
-      <c r="J14" s="77"/>
-      <c r="K14" s="85">
+      <c r="J14" s="73"/>
+      <c r="K14" s="81">
         <v>1</v>
       </c>
-      <c r="L14" s="70"/>
-      <c r="M14" s="77"/>
-      <c r="N14" s="85">
+      <c r="L14" s="66"/>
+      <c r="M14" s="73"/>
+      <c r="N14" s="81">
         <v>21</v>
       </c>
-      <c r="O14" s="70"/>
+      <c r="O14" s="66"/>
       <c r="P14" s="31"/>
-      <c r="Q14" s="77"/>
-      <c r="R14" s="85">
+      <c r="Q14" s="73"/>
+      <c r="R14" s="81">
         <v>1</v>
       </c>
-      <c r="S14" s="70"/>
-      <c r="T14" s="77"/>
-      <c r="U14" s="85">
+      <c r="S14" s="66"/>
+      <c r="T14" s="73"/>
+      <c r="U14" s="81">
         <v>21</v>
       </c>
-      <c r="V14" s="70"/>
+      <c r="V14" s="66"/>
     </row>
     <row r="15" spans="1:22" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="28"/>
@@ -1975,27 +1972,27 @@
       <c r="F15" s="28"/>
       <c r="G15" s="28"/>
       <c r="H15" s="28"/>
-      <c r="J15" s="84"/>
-      <c r="K15" s="86">
+      <c r="J15" s="80"/>
+      <c r="K15" s="82">
         <v>2</v>
       </c>
-      <c r="L15" s="83"/>
-      <c r="M15" s="84"/>
-      <c r="N15" s="86">
+      <c r="L15" s="79"/>
+      <c r="M15" s="80"/>
+      <c r="N15" s="82">
         <v>22</v>
       </c>
-      <c r="O15" s="83"/>
+      <c r="O15" s="79"/>
       <c r="P15" s="31"/>
-      <c r="Q15" s="84"/>
-      <c r="R15" s="86">
+      <c r="Q15" s="80"/>
+      <c r="R15" s="82">
         <v>2</v>
       </c>
-      <c r="S15" s="83"/>
-      <c r="T15" s="84"/>
-      <c r="U15" s="86">
+      <c r="S15" s="79"/>
+      <c r="T15" s="80"/>
+      <c r="U15" s="82">
         <v>22</v>
       </c>
-      <c r="V15" s="83"/>
+      <c r="V15" s="79"/>
     </row>
     <row r="16" spans="1:22" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="28"/>
@@ -2006,27 +2003,27 @@
       <c r="F16" s="28"/>
       <c r="G16" s="28"/>
       <c r="H16" s="28"/>
-      <c r="J16" s="78"/>
-      <c r="K16" s="87">
+      <c r="J16" s="74"/>
+      <c r="K16" s="83">
         <v>3</v>
       </c>
-      <c r="L16" s="70"/>
-      <c r="M16" s="78"/>
-      <c r="N16" s="87">
+      <c r="L16" s="66"/>
+      <c r="M16" s="74"/>
+      <c r="N16" s="83">
         <v>23</v>
       </c>
-      <c r="O16" s="70"/>
+      <c r="O16" s="66"/>
       <c r="P16" s="31"/>
-      <c r="Q16" s="78"/>
-      <c r="R16" s="87">
+      <c r="Q16" s="74"/>
+      <c r="R16" s="83">
         <v>3</v>
       </c>
-      <c r="S16" s="70"/>
-      <c r="T16" s="78"/>
-      <c r="U16" s="87">
+      <c r="S16" s="66"/>
+      <c r="T16" s="74"/>
+      <c r="U16" s="83">
         <v>23</v>
       </c>
-      <c r="V16" s="70"/>
+      <c r="V16" s="66"/>
     </row>
     <row r="17" spans="1:22" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="28"/>
@@ -2037,27 +2034,27 @@
       <c r="F17" s="28"/>
       <c r="G17" s="28"/>
       <c r="H17" s="28"/>
-      <c r="J17" s="84"/>
-      <c r="K17" s="86">
+      <c r="J17" s="80"/>
+      <c r="K17" s="82">
         <v>4</v>
       </c>
-      <c r="L17" s="83"/>
-      <c r="M17" s="84"/>
-      <c r="N17" s="86">
+      <c r="L17" s="79"/>
+      <c r="M17" s="80"/>
+      <c r="N17" s="82">
         <v>24</v>
       </c>
-      <c r="O17" s="83"/>
+      <c r="O17" s="79"/>
       <c r="P17" s="31"/>
-      <c r="Q17" s="84"/>
-      <c r="R17" s="86">
+      <c r="Q17" s="80"/>
+      <c r="R17" s="82">
         <v>4</v>
       </c>
-      <c r="S17" s="83"/>
-      <c r="T17" s="84"/>
-      <c r="U17" s="86">
+      <c r="S17" s="79"/>
+      <c r="T17" s="80"/>
+      <c r="U17" s="82">
         <v>24</v>
       </c>
-      <c r="V17" s="83"/>
+      <c r="V17" s="79"/>
     </row>
     <row r="18" spans="1:22" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="28"/>
@@ -2068,27 +2065,27 @@
       <c r="F18" s="28"/>
       <c r="G18" s="28"/>
       <c r="H18" s="28"/>
-      <c r="J18" s="78"/>
-      <c r="K18" s="87">
+      <c r="J18" s="74"/>
+      <c r="K18" s="83">
         <v>5</v>
       </c>
-      <c r="L18" s="70"/>
-      <c r="M18" s="78"/>
-      <c r="N18" s="87">
+      <c r="L18" s="66"/>
+      <c r="M18" s="74"/>
+      <c r="N18" s="83">
         <v>25</v>
       </c>
-      <c r="O18" s="70"/>
+      <c r="O18" s="66"/>
       <c r="P18" s="31"/>
-      <c r="Q18" s="78"/>
-      <c r="R18" s="87">
+      <c r="Q18" s="74"/>
+      <c r="R18" s="83">
         <v>5</v>
       </c>
-      <c r="S18" s="70"/>
-      <c r="T18" s="78"/>
-      <c r="U18" s="87">
+      <c r="S18" s="66"/>
+      <c r="T18" s="74"/>
+      <c r="U18" s="83">
         <v>25</v>
       </c>
-      <c r="V18" s="70"/>
+      <c r="V18" s="66"/>
     </row>
     <row r="19" spans="1:22" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="28"/>
@@ -2099,27 +2096,27 @@
       <c r="F19" s="28"/>
       <c r="G19" s="28"/>
       <c r="H19" s="28"/>
-      <c r="J19" s="84"/>
-      <c r="K19" s="86">
+      <c r="J19" s="80"/>
+      <c r="K19" s="82">
         <v>6</v>
       </c>
-      <c r="L19" s="83"/>
-      <c r="M19" s="84"/>
-      <c r="N19" s="86">
+      <c r="L19" s="79"/>
+      <c r="M19" s="80"/>
+      <c r="N19" s="82">
         <v>26</v>
       </c>
-      <c r="O19" s="83"/>
+      <c r="O19" s="79"/>
       <c r="P19" s="31"/>
-      <c r="Q19" s="84"/>
-      <c r="R19" s="86">
+      <c r="Q19" s="80"/>
+      <c r="R19" s="82">
         <v>6</v>
       </c>
-      <c r="S19" s="83"/>
-      <c r="T19" s="84"/>
-      <c r="U19" s="86">
+      <c r="S19" s="79"/>
+      <c r="T19" s="80"/>
+      <c r="U19" s="82">
         <v>26</v>
       </c>
-      <c r="V19" s="83"/>
+      <c r="V19" s="79"/>
     </row>
     <row r="20" spans="1:22" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="28"/>
@@ -2130,27 +2127,27 @@
       <c r="F20" s="28"/>
       <c r="G20" s="28"/>
       <c r="H20" s="28"/>
-      <c r="J20" s="80"/>
-      <c r="K20" s="88">
+      <c r="J20" s="76"/>
+      <c r="K20" s="84">
         <v>7</v>
       </c>
-      <c r="L20" s="81"/>
-      <c r="M20" s="80"/>
-      <c r="N20" s="88">
+      <c r="L20" s="77"/>
+      <c r="M20" s="76"/>
+      <c r="N20" s="84">
         <v>27</v>
       </c>
-      <c r="O20" s="81"/>
+      <c r="O20" s="77"/>
       <c r="P20" s="31"/>
-      <c r="Q20" s="80"/>
-      <c r="R20" s="88">
+      <c r="Q20" s="76"/>
+      <c r="R20" s="84">
         <v>7</v>
       </c>
-      <c r="S20" s="81"/>
-      <c r="T20" s="80"/>
-      <c r="U20" s="88">
+      <c r="S20" s="77"/>
+      <c r="T20" s="76"/>
+      <c r="U20" s="84">
         <v>27</v>
       </c>
-      <c r="V20" s="81"/>
+      <c r="V20" s="77"/>
     </row>
     <row r="21" spans="1:22" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="28"/>
@@ -2161,255 +2158,252 @@
       <c r="F21" s="28"/>
       <c r="G21" s="28"/>
       <c r="H21" s="28"/>
-      <c r="J21" s="84"/>
-      <c r="K21" s="86">
+      <c r="J21" s="80"/>
+      <c r="K21" s="82">
         <v>8</v>
       </c>
-      <c r="L21" s="83"/>
-      <c r="M21" s="84"/>
-      <c r="N21" s="86">
+      <c r="L21" s="79"/>
+      <c r="M21" s="80"/>
+      <c r="N21" s="82">
         <v>28</v>
       </c>
-      <c r="O21" s="83"/>
+      <c r="O21" s="79"/>
       <c r="P21" s="31"/>
-      <c r="Q21" s="84"/>
-      <c r="R21" s="86">
+      <c r="Q21" s="80"/>
+      <c r="R21" s="82">
         <v>8</v>
       </c>
-      <c r="S21" s="83"/>
-      <c r="T21" s="84"/>
-      <c r="U21" s="86">
+      <c r="S21" s="79"/>
+      <c r="T21" s="80"/>
+      <c r="U21" s="82">
         <v>28</v>
       </c>
-      <c r="V21" s="83"/>
-    </row>
-    <row r="22" spans="1:22" ht="14.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="32"/>
-      <c r="B22" s="33"/>
-      <c r="C22" s="34"/>
-      <c r="D22" s="35"/>
-      <c r="E22" s="35"/>
-      <c r="F22" s="35"/>
-      <c r="G22" s="35"/>
-      <c r="H22" s="35"/>
-      <c r="J22" s="78"/>
-      <c r="K22" s="87">
+      <c r="V21" s="79"/>
+    </row>
+    <row r="22" spans="1:22" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="28"/>
+      <c r="B22" s="29"/>
+      <c r="C22" s="30"/>
+      <c r="D22" s="28"/>
+      <c r="E22" s="28"/>
+      <c r="F22" s="28"/>
+      <c r="G22" s="28"/>
+      <c r="H22" s="28"/>
+      <c r="J22" s="74"/>
+      <c r="K22" s="83">
         <v>9</v>
       </c>
-      <c r="L22" s="70"/>
-      <c r="M22" s="78"/>
-      <c r="N22" s="87">
+      <c r="L22" s="66"/>
+      <c r="M22" s="74"/>
+      <c r="N22" s="83">
         <v>29</v>
       </c>
-      <c r="O22" s="70"/>
+      <c r="O22" s="66"/>
       <c r="P22" s="31"/>
-      <c r="Q22" s="78"/>
-      <c r="R22" s="87">
+      <c r="Q22" s="74"/>
+      <c r="R22" s="83">
         <v>9</v>
       </c>
-      <c r="S22" s="70"/>
-      <c r="T22" s="78"/>
-      <c r="U22" s="87">
+      <c r="S22" s="66"/>
+      <c r="T22" s="74"/>
+      <c r="U22" s="83">
         <v>29</v>
       </c>
-      <c r="V22" s="70"/>
-    </row>
-    <row r="23" spans="1:22" ht="14.1" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="36" t="s">
+      <c r="V22" s="66"/>
+    </row>
+    <row r="23" spans="1:22" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="28"/>
+      <c r="B23" s="29"/>
+      <c r="C23" s="30"/>
+      <c r="D23" s="28"/>
+      <c r="E23" s="28"/>
+      <c r="F23" s="28"/>
+      <c r="G23" s="28"/>
+      <c r="H23" s="28"/>
+      <c r="J23" s="80"/>
+      <c r="K23" s="82">
+        <v>10</v>
+      </c>
+      <c r="L23" s="79"/>
+      <c r="M23" s="80"/>
+      <c r="N23" s="82">
         <v>30</v>
       </c>
-      <c r="B23" s="37"/>
-      <c r="C23" s="38"/>
-      <c r="D23" s="39"/>
-      <c r="E23" s="36"/>
-      <c r="F23" s="36"/>
-      <c r="G23" s="36"/>
-      <c r="H23" s="36"/>
-      <c r="J23" s="84"/>
-      <c r="K23" s="86">
+      <c r="O23" s="79"/>
+      <c r="P23" s="31"/>
+      <c r="Q23" s="80"/>
+      <c r="R23" s="82">
         <v>10</v>
       </c>
-      <c r="L23" s="83"/>
-      <c r="M23" s="84"/>
-      <c r="N23" s="86">
+      <c r="S23" s="79"/>
+      <c r="T23" s="80"/>
+      <c r="U23" s="82">
         <v>30</v>
       </c>
-      <c r="O23" s="83"/>
-      <c r="P23" s="31"/>
-      <c r="Q23" s="84"/>
-      <c r="R23" s="86">
-        <v>10</v>
-      </c>
-      <c r="S23" s="83"/>
-      <c r="T23" s="84"/>
-      <c r="U23" s="86">
+      <c r="V23" s="79"/>
+    </row>
+    <row r="24" spans="1:22" ht="14.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="32"/>
+      <c r="B24" s="32"/>
+      <c r="C24" s="33"/>
+      <c r="D24" s="32"/>
+      <c r="E24" s="32"/>
+      <c r="F24" s="32"/>
+      <c r="G24" s="32"/>
+      <c r="H24" s="32"/>
+      <c r="I24" s="89"/>
+      <c r="J24" s="74"/>
+      <c r="K24" s="83">
+        <v>11</v>
+      </c>
+      <c r="L24" s="66"/>
+      <c r="M24" s="74"/>
+      <c r="N24" s="83">
+        <v>31</v>
+      </c>
+      <c r="O24" s="66"/>
+      <c r="P24" s="31"/>
+      <c r="Q24" s="74"/>
+      <c r="R24" s="83">
+        <v>11</v>
+      </c>
+      <c r="S24" s="66"/>
+      <c r="T24" s="74"/>
+      <c r="U24" s="83">
+        <v>31</v>
+      </c>
+      <c r="V24" s="66"/>
+    </row>
+    <row r="25" spans="1:22" ht="14.1" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="28" t="s">
         <v>30</v>
       </c>
-      <c r="V23" s="83"/>
-    </row>
-    <row r="24" spans="1:22" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="28" t="s">
-        <v>31</v>
-      </c>
-      <c r="B24" s="29"/>
-      <c r="C24" s="40"/>
-      <c r="D24" s="30"/>
-      <c r="E24" s="28"/>
-      <c r="F24" s="28"/>
-      <c r="G24" s="28"/>
-      <c r="H24" s="28"/>
-      <c r="J24" s="78"/>
-      <c r="K24" s="87">
-        <v>11</v>
-      </c>
-      <c r="L24" s="70"/>
-      <c r="M24" s="78"/>
-      <c r="N24" s="87">
-        <v>31</v>
-      </c>
-      <c r="O24" s="70"/>
-      <c r="P24" s="31"/>
-      <c r="Q24" s="78"/>
-      <c r="R24" s="87">
-        <v>11</v>
-      </c>
-      <c r="S24" s="70"/>
-      <c r="T24" s="78"/>
-      <c r="U24" s="87">
-        <v>31</v>
-      </c>
-      <c r="V24" s="70"/>
-    </row>
-    <row r="25" spans="1:22" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="28" t="s">
-        <v>32</v>
-      </c>
       <c r="B25" s="29"/>
-      <c r="C25" s="41"/>
+      <c r="C25" s="35"/>
       <c r="D25" s="30"/>
       <c r="E25" s="28"/>
       <c r="F25" s="28"/>
       <c r="G25" s="28"/>
       <c r="H25" s="28"/>
-      <c r="J25" s="84"/>
-      <c r="K25" s="86">
+      <c r="J25" s="80"/>
+      <c r="K25" s="82">
         <v>12</v>
       </c>
-      <c r="L25" s="83"/>
-      <c r="M25" s="84"/>
-      <c r="N25" s="86">
+      <c r="L25" s="79"/>
+      <c r="M25" s="80"/>
+      <c r="N25" s="82">
         <v>32</v>
       </c>
-      <c r="O25" s="83"/>
+      <c r="O25" s="79"/>
       <c r="P25" s="31"/>
-      <c r="Q25" s="84"/>
-      <c r="R25" s="86">
+      <c r="Q25" s="80"/>
+      <c r="R25" s="82">
         <v>12</v>
       </c>
-      <c r="S25" s="83"/>
-      <c r="T25" s="84"/>
-      <c r="U25" s="86">
+      <c r="S25" s="79"/>
+      <c r="T25" s="80"/>
+      <c r="U25" s="82">
         <v>32</v>
       </c>
-      <c r="V25" s="83"/>
+      <c r="V25" s="79"/>
     </row>
     <row r="26" spans="1:22" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="28" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="B26" s="29"/>
-      <c r="C26" s="40"/>
+      <c r="C26" s="36"/>
       <c r="D26" s="30"/>
       <c r="E26" s="28"/>
       <c r="F26" s="28"/>
       <c r="G26" s="28"/>
       <c r="H26" s="28"/>
-      <c r="J26" s="78"/>
-      <c r="K26" s="87">
+      <c r="J26" s="74"/>
+      <c r="K26" s="83">
         <v>13</v>
       </c>
-      <c r="L26" s="70"/>
-      <c r="M26" s="78"/>
-      <c r="N26" s="87">
+      <c r="L26" s="66"/>
+      <c r="M26" s="74"/>
+      <c r="N26" s="83">
         <v>33</v>
       </c>
-      <c r="O26" s="70"/>
+      <c r="O26" s="66"/>
       <c r="P26" s="31"/>
-      <c r="Q26" s="78"/>
-      <c r="R26" s="87">
+      <c r="Q26" s="74"/>
+      <c r="R26" s="83">
         <v>13</v>
       </c>
-      <c r="S26" s="70"/>
-      <c r="T26" s="78"/>
-      <c r="U26" s="87">
+      <c r="S26" s="66"/>
+      <c r="T26" s="74"/>
+      <c r="U26" s="83">
         <v>33</v>
       </c>
-      <c r="V26" s="70"/>
+      <c r="V26" s="66"/>
     </row>
     <row r="27" spans="1:22" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="103" t="s">
+      <c r="A27" s="104" t="s">
+        <v>32</v>
+      </c>
+      <c r="B27" s="105"/>
+      <c r="C27" s="106"/>
+      <c r="D27" s="30" t="s">
         <v>33</v>
-      </c>
-      <c r="B27" s="104"/>
-      <c r="C27" s="105"/>
-      <c r="D27" s="30" t="s">
-        <v>34</v>
       </c>
       <c r="E27" s="29"/>
       <c r="F27" s="30"/>
       <c r="G27" s="29"/>
       <c r="H27" s="30"/>
-      <c r="J27" s="84"/>
-      <c r="K27" s="86">
+      <c r="J27" s="80"/>
+      <c r="K27" s="82">
         <v>14</v>
       </c>
-      <c r="L27" s="83"/>
-      <c r="M27" s="84"/>
-      <c r="N27" s="86">
+      <c r="L27" s="79"/>
+      <c r="M27" s="80"/>
+      <c r="N27" s="82">
         <v>34</v>
       </c>
-      <c r="O27" s="83"/>
+      <c r="O27" s="79"/>
       <c r="P27" s="31"/>
-      <c r="Q27" s="84"/>
-      <c r="R27" s="86">
+      <c r="Q27" s="80"/>
+      <c r="R27" s="82">
         <v>14</v>
       </c>
-      <c r="S27" s="83"/>
-      <c r="T27" s="84"/>
-      <c r="U27" s="86">
+      <c r="S27" s="79"/>
+      <c r="T27" s="80"/>
+      <c r="U27" s="82">
         <v>34</v>
       </c>
-      <c r="V27" s="83"/>
+      <c r="V27" s="79"/>
     </row>
     <row r="28" spans="1:22" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="J28" s="78"/>
-      <c r="K28" s="87">
+      <c r="J28" s="74"/>
+      <c r="K28" s="83">
         <v>15</v>
       </c>
-      <c r="L28" s="70"/>
-      <c r="M28" s="78"/>
-      <c r="N28" s="87">
+      <c r="L28" s="66"/>
+      <c r="M28" s="74"/>
+      <c r="N28" s="83">
         <v>35</v>
       </c>
-      <c r="O28" s="70"/>
+      <c r="O28" s="66"/>
       <c r="P28" s="31"/>
-      <c r="Q28" s="78"/>
-      <c r="R28" s="87">
+      <c r="Q28" s="74"/>
+      <c r="R28" s="83">
         <v>15</v>
       </c>
-      <c r="S28" s="70"/>
-      <c r="T28" s="78"/>
-      <c r="U28" s="87">
+      <c r="S28" s="66"/>
+      <c r="T28" s="74"/>
+      <c r="U28" s="83">
         <v>35</v>
       </c>
-      <c r="V28" s="70"/>
+      <c r="V28" s="66"/>
     </row>
     <row r="29" spans="1:22" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="28" t="s">
         <v>24</v>
       </c>
       <c r="B29" s="29" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C29" s="30"/>
       <c r="D29" s="28" t="s">
@@ -2427,27 +2421,27 @@
       <c r="H29" s="28" t="s">
         <v>29</v>
       </c>
-      <c r="J29" s="84"/>
-      <c r="K29" s="86">
+      <c r="J29" s="80"/>
+      <c r="K29" s="82">
         <v>16</v>
       </c>
-      <c r="L29" s="83"/>
-      <c r="M29" s="84"/>
-      <c r="N29" s="86">
+      <c r="L29" s="79"/>
+      <c r="M29" s="80"/>
+      <c r="N29" s="82">
         <v>36</v>
       </c>
-      <c r="O29" s="83"/>
+      <c r="O29" s="79"/>
       <c r="P29" s="31"/>
-      <c r="Q29" s="84"/>
-      <c r="R29" s="86">
+      <c r="Q29" s="80"/>
+      <c r="R29" s="82">
         <v>16</v>
       </c>
-      <c r="S29" s="83"/>
-      <c r="T29" s="84"/>
-      <c r="U29" s="86">
+      <c r="S29" s="79"/>
+      <c r="T29" s="80"/>
+      <c r="U29" s="82">
         <v>36</v>
       </c>
-      <c r="V29" s="83"/>
+      <c r="V29" s="79"/>
     </row>
     <row r="30" spans="1:22" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="28"/>
@@ -2458,27 +2452,27 @@
       <c r="F30" s="28"/>
       <c r="G30" s="28"/>
       <c r="H30" s="28"/>
-      <c r="J30" s="80"/>
-      <c r="K30" s="88">
+      <c r="J30" s="76"/>
+      <c r="K30" s="84">
         <v>17</v>
       </c>
-      <c r="L30" s="81"/>
-      <c r="M30" s="80"/>
-      <c r="N30" s="88">
+      <c r="L30" s="77"/>
+      <c r="M30" s="76"/>
+      <c r="N30" s="84">
         <v>37</v>
       </c>
-      <c r="O30" s="81"/>
+      <c r="O30" s="77"/>
       <c r="P30" s="31"/>
-      <c r="Q30" s="80"/>
-      <c r="R30" s="88">
+      <c r="Q30" s="76"/>
+      <c r="R30" s="84">
         <v>17</v>
       </c>
-      <c r="S30" s="81"/>
-      <c r="T30" s="80"/>
-      <c r="U30" s="88">
+      <c r="S30" s="77"/>
+      <c r="T30" s="76"/>
+      <c r="U30" s="84">
         <v>37</v>
       </c>
-      <c r="V30" s="81"/>
+      <c r="V30" s="77"/>
     </row>
     <row r="31" spans="1:22" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="28"/>
@@ -2489,27 +2483,27 @@
       <c r="F31" s="28"/>
       <c r="G31" s="28"/>
       <c r="H31" s="28"/>
-      <c r="J31" s="80"/>
-      <c r="K31" s="88">
+      <c r="J31" s="76"/>
+      <c r="K31" s="84">
         <v>18</v>
       </c>
-      <c r="L31" s="81"/>
-      <c r="M31" s="80"/>
-      <c r="N31" s="88">
+      <c r="L31" s="77"/>
+      <c r="M31" s="76"/>
+      <c r="N31" s="84">
         <v>38</v>
       </c>
-      <c r="O31" s="81"/>
+      <c r="O31" s="77"/>
       <c r="P31" s="31"/>
-      <c r="Q31" s="80"/>
-      <c r="R31" s="88">
+      <c r="Q31" s="76"/>
+      <c r="R31" s="84">
         <v>18</v>
       </c>
-      <c r="S31" s="81"/>
-      <c r="T31" s="80"/>
-      <c r="U31" s="88">
+      <c r="S31" s="77"/>
+      <c r="T31" s="76"/>
+      <c r="U31" s="84">
         <v>38</v>
       </c>
-      <c r="V31" s="81"/>
+      <c r="V31" s="77"/>
     </row>
     <row r="32" spans="1:22" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="28"/>
@@ -2520,29 +2514,29 @@
       <c r="F32" s="28"/>
       <c r="G32" s="28"/>
       <c r="H32" s="28"/>
-      <c r="J32" s="80"/>
-      <c r="K32" s="88">
+      <c r="J32" s="76"/>
+      <c r="K32" s="84">
         <v>19</v>
       </c>
-      <c r="L32" s="81"/>
-      <c r="M32" s="80"/>
-      <c r="N32" s="88">
+      <c r="L32" s="77"/>
+      <c r="M32" s="76"/>
+      <c r="N32" s="84">
         <v>39</v>
       </c>
-      <c r="O32" s="81"/>
+      <c r="O32" s="77"/>
       <c r="P32" s="31"/>
-      <c r="Q32" s="80"/>
-      <c r="R32" s="88">
+      <c r="Q32" s="76"/>
+      <c r="R32" s="84">
         <v>19</v>
       </c>
-      <c r="S32" s="81"/>
-      <c r="T32" s="80"/>
-      <c r="U32" s="88">
+      <c r="S32" s="77"/>
+      <c r="T32" s="76"/>
+      <c r="U32" s="84">
         <v>39</v>
       </c>
-      <c r="V32" s="81"/>
-    </row>
-    <row r="33" spans="1:22" ht="14.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="V32" s="77"/>
+    </row>
+    <row r="33" spans="1:24" ht="14.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A33" s="28"/>
       <c r="B33" s="29"/>
       <c r="C33" s="30"/>
@@ -2551,29 +2545,29 @@
       <c r="F33" s="28"/>
       <c r="G33" s="28"/>
       <c r="H33" s="28"/>
-      <c r="J33" s="79"/>
-      <c r="K33" s="89">
+      <c r="J33" s="75"/>
+      <c r="K33" s="85">
         <v>20</v>
       </c>
-      <c r="L33" s="71"/>
-      <c r="M33" s="79"/>
-      <c r="N33" s="89">
+      <c r="L33" s="67"/>
+      <c r="M33" s="75"/>
+      <c r="N33" s="85">
         <v>40</v>
       </c>
-      <c r="O33" s="71"/>
+      <c r="O33" s="67"/>
       <c r="P33" s="31"/>
-      <c r="Q33" s="79"/>
-      <c r="R33" s="89">
+      <c r="Q33" s="75"/>
+      <c r="R33" s="85">
         <v>20</v>
       </c>
-      <c r="S33" s="71"/>
-      <c r="T33" s="79"/>
-      <c r="U33" s="89">
+      <c r="S33" s="67"/>
+      <c r="T33" s="75"/>
+      <c r="U33" s="85">
         <v>40</v>
       </c>
-      <c r="V33" s="71"/>
-    </row>
-    <row r="34" spans="1:22" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="V33" s="67"/>
+    </row>
+    <row r="34" spans="1:24" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="28"/>
       <c r="B34" s="29"/>
       <c r="C34" s="30"/>
@@ -2596,7 +2590,7 @@
       <c r="U34" s="31"/>
       <c r="V34" s="31"/>
     </row>
-    <row r="35" spans="1:22" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:24" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="28"/>
       <c r="B35" s="29"/>
       <c r="C35" s="30"/>
@@ -2619,7 +2613,7 @@
       <c r="U35" s="31"/>
       <c r="V35" s="31"/>
     </row>
-    <row r="36" spans="1:22" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:24" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="28"/>
       <c r="B36" s="29"/>
       <c r="C36" s="30"/>
@@ -2642,7 +2636,7 @@
       <c r="U36" s="31"/>
       <c r="V36" s="31"/>
     </row>
-    <row r="37" spans="1:22" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:24" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="28"/>
       <c r="B37" s="29"/>
       <c r="C37" s="30"/>
@@ -2665,7 +2659,7 @@
       <c r="U37" s="31"/>
       <c r="V37" s="31"/>
     </row>
-    <row r="38" spans="1:22" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:24" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="28"/>
       <c r="B38" s="29"/>
       <c r="C38" s="30"/>
@@ -2688,15 +2682,15 @@
       <c r="U38" s="31"/>
       <c r="V38" s="31"/>
     </row>
-    <row r="39" spans="1:22" ht="14.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="35"/>
-      <c r="B39" s="33"/>
-      <c r="C39" s="34"/>
-      <c r="D39" s="35"/>
-      <c r="E39" s="35"/>
-      <c r="F39" s="35"/>
-      <c r="G39" s="35"/>
-      <c r="H39" s="35"/>
+    <row r="39" spans="1:24" ht="14.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="28"/>
+      <c r="B39" s="29"/>
+      <c r="C39" s="30"/>
+      <c r="D39" s="28"/>
+      <c r="E39" s="28"/>
+      <c r="F39" s="28"/>
+      <c r="G39" s="28"/>
+      <c r="H39" s="28"/>
       <c r="J39" s="31"/>
       <c r="K39" s="31"/>
       <c r="L39" s="31"/>
@@ -2711,213 +2705,212 @@
       <c r="U39" s="31"/>
       <c r="V39" s="31"/>
     </row>
-    <row r="40" spans="1:22" ht="14.1" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A40" s="36" t="s">
-        <v>30</v>
-      </c>
-      <c r="B40" s="37"/>
-      <c r="C40" s="38"/>
-      <c r="D40" s="39"/>
-      <c r="E40" s="36"/>
-      <c r="F40" s="36"/>
-      <c r="G40" s="36"/>
-      <c r="H40" s="36"/>
-      <c r="J40" s="111" t="s">
+    <row r="40" spans="1:24" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A40" s="28"/>
+      <c r="B40" s="29"/>
+      <c r="C40" s="30"/>
+      <c r="D40" s="28"/>
+      <c r="E40" s="28"/>
+      <c r="F40" s="28"/>
+      <c r="G40" s="28"/>
+      <c r="H40" s="28"/>
+      <c r="J40" s="110" t="s">
+        <v>35</v>
+      </c>
+      <c r="K40" s="108"/>
+      <c r="L40" s="109"/>
+      <c r="M40" s="38"/>
+      <c r="N40" s="108" t="s">
         <v>36</v>
       </c>
-      <c r="K40" s="107"/>
-      <c r="L40" s="108"/>
-      <c r="M40" s="42"/>
-      <c r="N40" s="107" t="s">
+      <c r="O40" s="39"/>
+      <c r="P40" s="40"/>
+      <c r="Q40" s="107" t="s">
         <v>37</v>
       </c>
-      <c r="O40" s="43"/>
-      <c r="P40" s="44"/>
-      <c r="Q40" s="110" t="s">
-        <v>38</v>
-      </c>
-      <c r="R40" s="107"/>
-      <c r="S40" s="108"/>
-      <c r="T40" s="42"/>
-      <c r="U40" s="107" t="s">
-        <v>37</v>
-      </c>
-      <c r="V40" s="45"/>
-    </row>
-    <row r="41" spans="1:22" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A41" s="28" t="s">
-        <v>31</v>
-      </c>
-      <c r="B41" s="29"/>
-      <c r="C41" s="40"/>
-      <c r="D41" s="30"/>
-      <c r="E41" s="28"/>
-      <c r="F41" s="28"/>
-      <c r="G41" s="28"/>
-      <c r="H41" s="28"/>
-      <c r="J41" s="109"/>
-      <c r="K41" s="94"/>
-      <c r="L41" s="95"/>
+      <c r="R40" s="108"/>
+      <c r="S40" s="109"/>
+      <c r="T40" s="38"/>
+      <c r="U40" s="108" t="s">
+        <v>36</v>
+      </c>
+      <c r="V40" s="41"/>
+    </row>
+    <row r="41" spans="1:24" ht="14.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="87"/>
+      <c r="B41" s="32"/>
+      <c r="C41" s="88"/>
+      <c r="D41" s="88"/>
+      <c r="E41" s="87"/>
+      <c r="F41" s="87"/>
+      <c r="G41" s="87"/>
+      <c r="H41" s="87"/>
+      <c r="J41" s="112"/>
+      <c r="K41" s="95"/>
+      <c r="L41" s="96"/>
       <c r="M41" s="21"/>
-      <c r="N41" s="94"/>
+      <c r="N41" s="95"/>
       <c r="O41" s="22"/>
       <c r="P41" s="9"/>
-      <c r="Q41" s="93"/>
-      <c r="R41" s="94"/>
-      <c r="S41" s="95"/>
+      <c r="Q41" s="94"/>
+      <c r="R41" s="95"/>
+      <c r="S41" s="96"/>
       <c r="T41" s="21"/>
-      <c r="U41" s="94"/>
-      <c r="V41" s="46"/>
-    </row>
-    <row r="42" spans="1:22" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A42" s="28" t="s">
-        <v>32</v>
-      </c>
-      <c r="B42" s="29"/>
-      <c r="C42" s="40"/>
-      <c r="D42" s="30"/>
-      <c r="E42" s="28"/>
-      <c r="F42" s="28"/>
-      <c r="G42" s="28"/>
-      <c r="H42" s="28"/>
-      <c r="J42" s="97" t="s">
-        <v>39</v>
-      </c>
-      <c r="K42" s="91"/>
-      <c r="L42" s="92"/>
+      <c r="U41" s="95"/>
+      <c r="V41" s="42"/>
+    </row>
+    <row r="42" spans="1:24" ht="14.1" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="A42" s="86" t="s">
+        <v>30</v>
+      </c>
+      <c r="B42" s="53"/>
+      <c r="C42" s="54"/>
+      <c r="D42" s="55"/>
+      <c r="E42" s="86"/>
+      <c r="F42" s="86"/>
+      <c r="G42" s="86"/>
+      <c r="H42" s="86"/>
+      <c r="J42" s="98" t="s">
+        <v>38</v>
+      </c>
+      <c r="K42" s="92"/>
+      <c r="L42" s="93"/>
       <c r="M42" s="10"/>
-      <c r="N42" s="91" t="s">
-        <v>37</v>
+      <c r="N42" s="92" t="s">
+        <v>36</v>
       </c>
       <c r="O42" s="20"/>
       <c r="P42" s="9"/>
-      <c r="Q42" s="90" t="s">
-        <v>39</v>
-      </c>
-      <c r="R42" s="91"/>
-      <c r="S42" s="92"/>
+      <c r="Q42" s="91" t="s">
+        <v>38</v>
+      </c>
+      <c r="R42" s="92"/>
+      <c r="S42" s="93"/>
       <c r="T42" s="10"/>
-      <c r="U42" s="91" t="s">
-        <v>37</v>
-      </c>
-      <c r="V42" s="47"/>
-    </row>
-    <row r="43" spans="1:22" ht="14.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="35" t="s">
-        <v>28</v>
-      </c>
-      <c r="B43" s="48"/>
-      <c r="C43" s="41"/>
+      <c r="U42" s="92" t="s">
+        <v>36</v>
+      </c>
+      <c r="V42" s="43"/>
+    </row>
+    <row r="43" spans="1:24" ht="14.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="34" t="s">
+        <v>31</v>
+      </c>
+      <c r="B43" s="44"/>
+      <c r="C43" s="37"/>
       <c r="D43" s="30"/>
       <c r="E43" s="28"/>
       <c r="F43" s="28"/>
       <c r="G43" s="28"/>
       <c r="H43" s="28"/>
-      <c r="J43" s="98"/>
-      <c r="K43" s="99"/>
-      <c r="L43" s="100"/>
+      <c r="J43" s="99"/>
+      <c r="K43" s="100"/>
+      <c r="L43" s="101"/>
       <c r="M43" s="21"/>
-      <c r="N43" s="101"/>
+      <c r="N43" s="102"/>
       <c r="O43" s="22"/>
       <c r="P43" s="9"/>
-      <c r="Q43" s="102"/>
-      <c r="R43" s="99"/>
-      <c r="S43" s="100"/>
+      <c r="Q43" s="103"/>
+      <c r="R43" s="100"/>
+      <c r="S43" s="101"/>
       <c r="T43" s="21"/>
-      <c r="U43" s="101"/>
-      <c r="V43" s="46"/>
-    </row>
-    <row r="44" spans="1:22" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A44" s="103" t="s">
+      <c r="U43" s="102"/>
+      <c r="V43" s="42"/>
+    </row>
+    <row r="44" spans="1:24" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A44" s="104" t="s">
+        <v>32</v>
+      </c>
+      <c r="B44" s="105"/>
+      <c r="C44" s="106"/>
+      <c r="D44" s="30" t="s">
         <v>33</v>
-      </c>
-      <c r="B44" s="104"/>
-      <c r="C44" s="105"/>
-      <c r="D44" s="30" t="s">
-        <v>34</v>
       </c>
       <c r="E44" s="29"/>
       <c r="F44" s="30"/>
       <c r="G44" s="29"/>
       <c r="H44" s="30"/>
-      <c r="J44" s="106" t="s">
-        <v>40</v>
-      </c>
-      <c r="K44" s="107"/>
-      <c r="L44" s="107"/>
-      <c r="M44" s="107"/>
-      <c r="N44" s="107"/>
-      <c r="O44" s="108"/>
-      <c r="P44" s="44"/>
-      <c r="Q44" s="110" t="s">
-        <v>41</v>
-      </c>
-      <c r="R44" s="107"/>
-      <c r="S44" s="108"/>
-      <c r="T44" s="42"/>
-      <c r="U44" s="107" t="s">
-        <v>37</v>
-      </c>
-      <c r="V44" s="45"/>
-    </row>
-    <row r="45" spans="1:22" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A45" s="49"/>
-      <c r="B45" s="49"/>
-      <c r="C45" s="49"/>
+      <c r="J44" s="110" t="s">
+        <v>57</v>
+      </c>
+      <c r="K44" s="108"/>
+      <c r="L44" s="108"/>
+      <c r="M44" s="108"/>
+      <c r="N44" s="108"/>
+      <c r="O44" s="109"/>
+      <c r="P44" s="40"/>
+      <c r="Q44" s="107" t="s">
+        <v>39</v>
+      </c>
+      <c r="R44" s="108"/>
+      <c r="S44" s="109"/>
+      <c r="T44" s="38"/>
+      <c r="U44" s="108" t="s">
+        <v>36</v>
+      </c>
+      <c r="V44" s="41"/>
+    </row>
+    <row r="45" spans="1:24" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A45" s="45"/>
+      <c r="B45" s="45"/>
+      <c r="C45" s="45"/>
       <c r="D45" s="31"/>
       <c r="E45" s="31"/>
       <c r="F45" s="31"/>
       <c r="G45" s="31"/>
       <c r="H45" s="31"/>
-      <c r="J45" s="109"/>
-      <c r="K45" s="94"/>
-      <c r="L45" s="94"/>
-      <c r="M45" s="94"/>
-      <c r="N45" s="94"/>
-      <c r="O45" s="95"/>
+      <c r="J45" s="111" t="s">
+        <v>58</v>
+      </c>
+      <c r="K45" s="95"/>
+      <c r="L45" s="95"/>
+      <c r="M45" s="95"/>
+      <c r="N45" s="95"/>
+      <c r="O45" s="96"/>
       <c r="P45" s="9"/>
-      <c r="Q45" s="93"/>
-      <c r="R45" s="94"/>
-      <c r="S45" s="95"/>
+      <c r="Q45" s="94"/>
+      <c r="R45" s="95"/>
+      <c r="S45" s="96"/>
       <c r="T45" s="21"/>
-      <c r="U45" s="94"/>
-      <c r="V45" s="46"/>
-    </row>
-    <row r="46" spans="1:22" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="J46" s="50"/>
+      <c r="U45" s="95"/>
+      <c r="V45" s="42"/>
+      <c r="X45" s="90"/>
+    </row>
+    <row r="46" spans="1:24" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J46" s="46"/>
       <c r="K46" s="19"/>
       <c r="L46" s="19"/>
       <c r="M46" s="19"/>
       <c r="N46" s="19"/>
       <c r="O46" s="19"/>
       <c r="P46" s="20"/>
-      <c r="Q46" s="90" t="s">
-        <v>39</v>
-      </c>
-      <c r="R46" s="91"/>
-      <c r="S46" s="92"/>
+      <c r="Q46" s="91" t="s">
+        <v>38</v>
+      </c>
+      <c r="R46" s="92"/>
+      <c r="S46" s="93"/>
       <c r="T46" s="19"/>
-      <c r="U46" s="91" t="s">
-        <v>37</v>
-      </c>
-      <c r="V46" s="47"/>
-    </row>
-    <row r="47" spans="1:22" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="U46" s="92" t="s">
+        <v>36</v>
+      </c>
+      <c r="V46" s="43"/>
+    </row>
+    <row r="47" spans="1:24" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B47" t="s">
+        <v>40</v>
+      </c>
+      <c r="C47" s="97" t="s">
+        <v>41</v>
+      </c>
+      <c r="D47" s="97"/>
+      <c r="E47" s="97" t="s">
         <v>42</v>
       </c>
-      <c r="C47" s="96" t="s">
+      <c r="F47" s="97"/>
+      <c r="G47" s="97"/>
+      <c r="H47" s="97"/>
+      <c r="J47" s="47" t="s">
         <v>43</v>
-      </c>
-      <c r="D47" s="96"/>
-      <c r="E47" s="96" t="s">
-        <v>44</v>
-      </c>
-      <c r="F47" s="96"/>
-      <c r="G47" s="96"/>
-      <c r="H47" s="96"/>
-      <c r="J47" s="51" t="s">
-        <v>45</v>
       </c>
       <c r="K47" s="26"/>
       <c r="L47" s="26"/>
@@ -2925,99 +2918,99 @@
       <c r="N47" s="26"/>
       <c r="O47" s="26"/>
       <c r="P47" s="27"/>
-      <c r="Q47" s="93"/>
-      <c r="R47" s="94"/>
-      <c r="S47" s="95"/>
+      <c r="Q47" s="94"/>
+      <c r="R47" s="95"/>
+      <c r="S47" s="96"/>
       <c r="T47" s="26"/>
-      <c r="U47" s="94"/>
-      <c r="V47" s="52"/>
-    </row>
-    <row r="48" spans="1:22" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="U47" s="95"/>
+      <c r="V47" s="48"/>
+    </row>
+    <row r="48" spans="1:24" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A48" s="28">
         <v>1</v>
       </c>
       <c r="B48" s="29"/>
       <c r="C48" s="29"/>
       <c r="D48" s="30"/>
-      <c r="E48" s="40"/>
-      <c r="F48" s="40"/>
-      <c r="G48" s="40"/>
+      <c r="E48" s="36"/>
+      <c r="F48" s="36"/>
+      <c r="G48" s="36"/>
       <c r="H48" s="30"/>
-      <c r="J48" s="53" t="s">
+      <c r="J48" s="49" t="s">
         <v>24</v>
       </c>
       <c r="K48" s="27"/>
-      <c r="L48" s="54"/>
-      <c r="M48" s="54"/>
-      <c r="N48" s="54"/>
-      <c r="O48" s="55"/>
+      <c r="L48" s="50"/>
+      <c r="M48" s="50"/>
+      <c r="N48" s="50"/>
+      <c r="O48" s="51"/>
       <c r="P48" s="27"/>
-      <c r="Q48" s="54"/>
-      <c r="R48" s="54"/>
-      <c r="S48" s="54"/>
-      <c r="T48" s="55"/>
+      <c r="Q48" s="50"/>
+      <c r="R48" s="50"/>
+      <c r="S48" s="50"/>
+      <c r="T48" s="51"/>
       <c r="U48" s="27"/>
-      <c r="V48" s="56"/>
+      <c r="V48" s="52"/>
     </row>
     <row r="49" spans="1:22" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A49" s="28">
         <v>2</v>
       </c>
-      <c r="B49" s="57"/>
+      <c r="B49" s="53"/>
       <c r="C49" s="29"/>
       <c r="D49" s="30"/>
-      <c r="E49" s="58"/>
-      <c r="F49" s="58"/>
-      <c r="G49" s="58"/>
-      <c r="H49" s="59"/>
-      <c r="J49" s="60" t="s">
-        <v>46</v>
+      <c r="E49" s="54"/>
+      <c r="F49" s="54"/>
+      <c r="G49" s="54"/>
+      <c r="H49" s="55"/>
+      <c r="J49" s="56" t="s">
+        <v>44</v>
       </c>
       <c r="K49" s="18"/>
       <c r="L49" s="4"/>
       <c r="M49" s="4"/>
       <c r="N49" s="4"/>
-      <c r="O49" s="61"/>
+      <c r="O49" s="57"/>
       <c r="P49" s="18"/>
       <c r="Q49" s="4"/>
       <c r="R49" s="4"/>
       <c r="S49" s="4"/>
-      <c r="T49" s="61"/>
+      <c r="T49" s="57"/>
       <c r="U49" s="18"/>
-      <c r="V49" s="62"/>
+      <c r="V49" s="58"/>
     </row>
     <row r="50" spans="1:22" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B50" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C50" s="31"/>
       <c r="D50" s="31"/>
-      <c r="J50" s="60" t="s">
+      <c r="J50" s="56" t="s">
         <v>26</v>
       </c>
       <c r="K50" s="18"/>
       <c r="L50" s="4"/>
       <c r="M50" s="4"/>
       <c r="N50" s="4"/>
-      <c r="O50" s="61"/>
+      <c r="O50" s="57"/>
       <c r="P50" s="18"/>
       <c r="Q50" s="4"/>
       <c r="R50" s="4"/>
       <c r="S50" s="4"/>
-      <c r="T50" s="61"/>
+      <c r="T50" s="57"/>
       <c r="U50" s="18"/>
-      <c r="V50" s="62"/>
+      <c r="V50" s="58"/>
     </row>
     <row r="51" spans="1:22" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B51" s="29"/>
       <c r="C51" s="29"/>
       <c r="D51" s="30"/>
-      <c r="E51" s="40"/>
-      <c r="F51" s="40"/>
-      <c r="G51" s="40"/>
+      <c r="E51" s="36"/>
+      <c r="F51" s="36"/>
+      <c r="G51" s="36"/>
       <c r="H51" s="30"/>
-      <c r="J51" s="60" t="s">
-        <v>35</v>
+      <c r="J51" s="56" t="s">
+        <v>34</v>
       </c>
       <c r="K51" s="9"/>
       <c r="L51" s="9"/>
@@ -3030,88 +3023,88 @@
       <c r="S51" s="9"/>
       <c r="T51" s="9"/>
       <c r="U51" s="9"/>
-      <c r="V51" s="46"/>
+      <c r="V51" s="42"/>
     </row>
     <row r="52" spans="1:22" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B52" s="57"/>
-      <c r="C52" s="57"/>
-      <c r="D52" s="59"/>
-      <c r="E52" s="58"/>
-      <c r="F52" s="58"/>
-      <c r="G52" s="58"/>
-      <c r="H52" s="59"/>
-      <c r="J52" s="60" t="s">
+      <c r="B52" s="53"/>
+      <c r="C52" s="53"/>
+      <c r="D52" s="55"/>
+      <c r="E52" s="54"/>
+      <c r="F52" s="54"/>
+      <c r="G52" s="54"/>
+      <c r="H52" s="55"/>
+      <c r="J52" s="56" t="s">
         <v>24</v>
       </c>
       <c r="K52" s="18"/>
       <c r="L52" s="4"/>
       <c r="M52" s="4"/>
       <c r="N52" s="4"/>
-      <c r="O52" s="61"/>
+      <c r="O52" s="57"/>
       <c r="P52" s="18"/>
       <c r="Q52" s="4"/>
       <c r="R52" s="4"/>
       <c r="S52" s="4"/>
-      <c r="T52" s="61"/>
+      <c r="T52" s="57"/>
       <c r="U52" s="18"/>
-      <c r="V52" s="62"/>
+      <c r="V52" s="58"/>
     </row>
     <row r="53" spans="1:22" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B53" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C53" s="31"/>
       <c r="D53" s="31"/>
-      <c r="J53" s="60" t="s">
-        <v>46</v>
+      <c r="J53" s="56" t="s">
+        <v>44</v>
       </c>
       <c r="K53" s="18"/>
       <c r="L53" s="4"/>
       <c r="M53" s="4"/>
       <c r="N53" s="4"/>
-      <c r="O53" s="61"/>
+      <c r="O53" s="57"/>
       <c r="P53" s="18"/>
       <c r="Q53" s="4"/>
       <c r="R53" s="4"/>
       <c r="S53" s="4"/>
-      <c r="T53" s="61"/>
+      <c r="T53" s="57"/>
       <c r="U53" s="18"/>
-      <c r="V53" s="62"/>
+      <c r="V53" s="58"/>
     </row>
     <row r="54" spans="1:22" ht="14.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B54" s="29"/>
       <c r="C54" s="29"/>
       <c r="D54" s="30"/>
-      <c r="E54" s="40"/>
-      <c r="F54" s="40"/>
-      <c r="G54" s="40"/>
+      <c r="E54" s="36"/>
+      <c r="F54" s="36"/>
+      <c r="G54" s="36"/>
       <c r="H54" s="30"/>
-      <c r="J54" s="63" t="s">
+      <c r="J54" s="59" t="s">
         <v>26</v>
       </c>
-      <c r="K54" s="64"/>
-      <c r="L54" s="65"/>
-      <c r="M54" s="65"/>
-      <c r="N54" s="65"/>
-      <c r="O54" s="66"/>
-      <c r="P54" s="64"/>
-      <c r="Q54" s="65"/>
-      <c r="R54" s="65"/>
-      <c r="S54" s="65"/>
-      <c r="T54" s="66"/>
-      <c r="U54" s="64"/>
-      <c r="V54" s="67"/>
-    </row>
-    <row r="55" spans="1:22" s="68" customFormat="1" ht="3.75" customHeight="1" x14ac:dyDescent="0.2"/>
+      <c r="K54" s="60"/>
+      <c r="L54" s="61"/>
+      <c r="M54" s="61"/>
+      <c r="N54" s="61"/>
+      <c r="O54" s="62"/>
+      <c r="P54" s="60"/>
+      <c r="Q54" s="61"/>
+      <c r="R54" s="61"/>
+      <c r="S54" s="61"/>
+      <c r="T54" s="62"/>
+      <c r="U54" s="60"/>
+      <c r="V54" s="63"/>
+    </row>
+    <row r="55" spans="1:22" s="64" customFormat="1" ht="3.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="56" spans="1:22" ht="8.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B56" s="5" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C56" s="5" t="s">
         <v>28</v>
       </c>
       <c r="D56" s="5" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="E56" s="5"/>
       <c r="F56" s="5"/>
@@ -3119,7 +3112,7 @@
         <v>29</v>
       </c>
       <c r="H56" s="5" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="I56" s="5"/>
       <c r="J56" s="5"/>
@@ -3127,15 +3120,15 @@
         <v>26</v>
       </c>
       <c r="L56" s="5" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="M56" s="5"/>
       <c r="N56" s="5"/>
       <c r="O56" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="P56" s="69" t="s">
-        <v>53</v>
+        <v>33</v>
+      </c>
+      <c r="P56" s="65" t="s">
+        <v>51</v>
       </c>
       <c r="Q56" s="5"/>
       <c r="R56" s="5"/>
@@ -3144,10 +3137,10 @@
     <row r="57" spans="1:22" ht="8.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B57" s="8"/>
       <c r="C57" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="D57" s="69" t="s">
-        <v>54</v>
+        <v>44</v>
+      </c>
+      <c r="D57" s="65" t="s">
+        <v>52</v>
       </c>
       <c r="E57" s="8"/>
       <c r="F57" s="8"/>
@@ -3155,7 +3148,7 @@
         <v>24</v>
       </c>
       <c r="H57" s="5" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="I57" s="8"/>
       <c r="J57" s="8"/>
@@ -3163,22 +3156,22 @@
         <v>27</v>
       </c>
       <c r="L57" s="5" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="M57" s="8"/>
       <c r="N57" s="8"/>
       <c r="O57" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="P57" s="69" t="s">
-        <v>58</v>
+        <v>55</v>
+      </c>
+      <c r="P57" s="65" t="s">
+        <v>56</v>
       </c>
       <c r="Q57" s="8"/>
       <c r="R57" s="8"/>
       <c r="S57" s="5"/>
     </row>
   </sheetData>
-  <mergeCells count="28">
+  <mergeCells count="29">
     <mergeCell ref="J12:O12"/>
     <mergeCell ref="Q12:V12"/>
     <mergeCell ref="L9:M9"/>
@@ -3204,9 +3197,10 @@
     <mergeCell ref="Q42:S43"/>
     <mergeCell ref="U42:U43"/>
     <mergeCell ref="A44:C44"/>
-    <mergeCell ref="J44:O45"/>
     <mergeCell ref="Q44:S45"/>
     <mergeCell ref="U44:U45"/>
+    <mergeCell ref="J44:O44"/>
+    <mergeCell ref="J45:O45"/>
   </mergeCells>
   <pageMargins left="0" right="0" top="0.39370078740157483" bottom="0.39370078740157483" header="0.51181102362204722" footer="0.51181102362204722"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>